<commit_message>
some clean up and added distance to df variable
</commit_message>
<xml_diff>
--- a/raw_data/metadata.xlsx
+++ b/raw_data/metadata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joegunn/Desktop/Projects/SMB_Fitness/raw_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F3929DB-3286-2F48-A493-9FEE7481C208}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F9DAEEE-4F87-7D43-A754-4865418393FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1620" yWindow="920" windowWidth="27640" windowHeight="16260" xr2:uid="{1D6D6247-8763-7240-99C2-409594371EA5}"/>
+    <workbookView xWindow="1160" yWindow="720" windowWidth="27640" windowHeight="16260" xr2:uid="{1D6D6247-8763-7240-99C2-409594371EA5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1047" uniqueCount="411">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1047" uniqueCount="412">
   <si>
     <t>sample_id</t>
   </si>
@@ -1269,6 +1269,9 @@
   </si>
   <si>
     <t>REF_20</t>
+  </si>
+  <si>
+    <t>dist_from_df</t>
   </si>
 </sst>
 </file>
@@ -1331,7 +1334,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1353,6 +1356,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1667,10 +1671,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16C20FF8-CFFA-9A48-91C2-CA4D661BB7BE}">
-  <dimension ref="A1:I137"/>
+  <dimension ref="A1:J137"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A112" workbookViewId="0">
-      <selection activeCell="D118" sqref="D118:D137"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1678,11 +1682,12 @@
     <col min="3" max="3" width="14.33203125" customWidth="1"/>
     <col min="4" max="4" width="16.33203125" customWidth="1"/>
     <col min="5" max="6" width="14.33203125" customWidth="1"/>
-    <col min="7" max="7" width="17.6640625" customWidth="1"/>
-    <col min="8" max="8" width="16.5" customWidth="1"/>
+    <col min="7" max="7" width="18.6640625" customWidth="1"/>
+    <col min="8" max="8" width="17.6640625" customWidth="1"/>
+    <col min="9" max="9" width="16.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1702,16 +1707,19 @@
         <v>164</v>
       </c>
       <c r="G1" s="5" t="s">
+        <v>411</v>
+      </c>
+      <c r="H1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="I1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="J1" s="5" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>43</v>
       </c>
@@ -1725,22 +1733,25 @@
         <v>275</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>165</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>165</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>159</v>
+        <v>166</v>
+      </c>
+      <c r="F2" s="2">
+        <v>4052386</v>
+      </c>
+      <c r="G2" s="9">
+        <v>1259.1600000000001</v>
       </c>
       <c r="H2" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="I2" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="I2" s="2" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J2" s="2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>44</v>
       </c>
@@ -1759,17 +1770,20 @@
       <c r="F3" s="2">
         <v>4052386</v>
       </c>
-      <c r="G3" s="2" t="s">
-        <v>159</v>
+      <c r="G3" s="9">
+        <v>1259.1600000000001</v>
       </c>
       <c r="H3" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="I3" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="I3" s="2" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J3" s="2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>45</v>
       </c>
@@ -1788,17 +1802,20 @@
       <c r="F4" s="2">
         <v>4051749</v>
       </c>
-      <c r="G4" s="2" t="s">
-        <v>159</v>
+      <c r="G4" s="9">
+        <v>1956.01</v>
       </c>
       <c r="H4" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="I4" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="I4" s="2" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J4" s="2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>46</v>
       </c>
@@ -1817,17 +1834,20 @@
       <c r="F5" s="2">
         <v>4051738</v>
       </c>
-      <c r="G5" s="2" t="s">
-        <v>159</v>
+      <c r="G5" s="9">
+        <v>1982.3899999999999</v>
       </c>
       <c r="H5" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="I5" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="I5" s="2" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J5" s="2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>47</v>
       </c>
@@ -1846,17 +1866,20 @@
       <c r="F6" s="2">
         <v>4051735</v>
       </c>
-      <c r="G6" s="2" t="s">
-        <v>159</v>
+      <c r="G6" s="9">
+        <v>1982.3899999999999</v>
       </c>
       <c r="H6" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="I6" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="I6" s="2" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J6" s="2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>48</v>
       </c>
@@ -1875,17 +1898,20 @@
       <c r="F7" s="2">
         <v>4051754</v>
       </c>
-      <c r="G7" s="2" t="s">
-        <v>159</v>
+      <c r="G7" s="9">
+        <v>2240.33</v>
       </c>
       <c r="H7" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="I7" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="I7" s="2" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J7" s="2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>49</v>
       </c>
@@ -1904,17 +1930,20 @@
       <c r="F8" s="2">
         <v>4052882</v>
       </c>
-      <c r="G8" s="2" t="s">
-        <v>159</v>
+      <c r="G8" s="9">
+        <v>681.94999999999993</v>
       </c>
       <c r="H8" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="I8" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="I8" s="2" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J8" s="2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>50</v>
       </c>
@@ -1933,17 +1962,20 @@
       <c r="F9" s="2">
         <v>4052702</v>
       </c>
-      <c r="G9" s="2" t="s">
-        <v>159</v>
+      <c r="G9" s="9">
+        <v>942.57999999999993</v>
       </c>
       <c r="H9" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="I9" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="I9" s="2" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J9" s="2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>51</v>
       </c>
@@ -1962,17 +1994,20 @@
       <c r="F10" s="2">
         <v>4051107</v>
       </c>
-      <c r="G10" s="2" t="s">
-        <v>159</v>
+      <c r="G10" s="9">
+        <v>4570.7700000000004</v>
       </c>
       <c r="H10" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="I10" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="I10" s="2" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J10" s="2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>52</v>
       </c>
@@ -1991,17 +2026,20 @@
       <c r="F11" s="2">
         <v>4053309</v>
       </c>
-      <c r="G11" s="2" t="s">
-        <v>159</v>
+      <c r="G11" s="9">
+        <v>0</v>
       </c>
       <c r="H11" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="I11" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="I11" s="2" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J11" s="2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>53</v>
       </c>
@@ -2020,17 +2058,20 @@
       <c r="F12" s="2">
         <v>4053309</v>
       </c>
-      <c r="G12" s="2" t="s">
-        <v>159</v>
+      <c r="G12" s="9">
+        <v>0</v>
       </c>
       <c r="H12" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="I12" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="I12" s="2" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J12" s="2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>54</v>
       </c>
@@ -2049,17 +2090,20 @@
       <c r="F13" s="2">
         <v>4052373</v>
       </c>
-      <c r="G13" s="2" t="s">
-        <v>159</v>
+      <c r="G13" s="9">
+        <v>1295.98</v>
       </c>
       <c r="H13" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="I13" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="I13" s="2" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J13" s="2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>55</v>
       </c>
@@ -2078,17 +2122,20 @@
       <c r="F14" s="2">
         <v>4051806</v>
       </c>
-      <c r="G14" s="2" t="s">
-        <v>159</v>
+      <c r="G14" s="9">
+        <v>2342.58</v>
       </c>
       <c r="H14" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="I14" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="I14" s="2" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J14" s="2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>56</v>
       </c>
@@ -2107,17 +2154,20 @@
       <c r="F15" s="2">
         <v>4050212</v>
       </c>
-      <c r="G15" s="2" t="s">
-        <v>159</v>
+      <c r="G15" s="9">
+        <v>5797.97</v>
       </c>
       <c r="H15" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="I15" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="I15" s="2" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J15" s="2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>57</v>
       </c>
@@ -2136,17 +2186,20 @@
       <c r="F16" s="2">
         <v>4050101</v>
       </c>
-      <c r="G16" s="2" t="s">
-        <v>159</v>
+      <c r="G16" s="9">
+        <v>5995.6500000000005</v>
       </c>
       <c r="H16" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="I16" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="I16" s="2" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J16" s="2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>58</v>
       </c>
@@ -2165,17 +2218,20 @@
       <c r="F17" s="2">
         <v>4050101</v>
       </c>
-      <c r="G17" s="2" t="s">
-        <v>159</v>
+      <c r="G17" s="9">
+        <v>5995.6500000000005</v>
       </c>
       <c r="H17" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="I17" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="I17" s="2" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J17" s="2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>59</v>
       </c>
@@ -2194,17 +2250,20 @@
       <c r="F18" s="2">
         <v>4052933</v>
       </c>
-      <c r="G18" s="2" t="s">
-        <v>159</v>
+      <c r="G18" s="9">
+        <v>622.92999999999995</v>
       </c>
       <c r="H18" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="I18" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="I18" s="2" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J18" s="2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>60</v>
       </c>
@@ -2223,17 +2282,20 @@
       <c r="F19" s="2">
         <v>4052818</v>
       </c>
-      <c r="G19" s="2" t="s">
-        <v>159</v>
+      <c r="G19" s="9">
+        <v>799.54</v>
       </c>
       <c r="H19" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="I19" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="I19" s="2" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J19" s="2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>61</v>
       </c>
@@ -2252,17 +2314,20 @@
       <c r="F20" s="2">
         <v>4051795</v>
       </c>
-      <c r="G20" s="2" t="s">
-        <v>159</v>
+      <c r="G20" s="9">
+        <v>3168.06</v>
       </c>
       <c r="H20" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="I20" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="I20" s="2" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J20" s="2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>62</v>
       </c>
@@ -2281,17 +2346,20 @@
       <c r="F21" s="2">
         <v>4051716</v>
       </c>
-      <c r="G21" s="2" t="s">
-        <v>159</v>
+      <c r="G21" s="9">
+        <v>2078.0299999999997</v>
       </c>
       <c r="H21" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="I21" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="I21" s="2" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J21" s="2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>63</v>
       </c>
@@ -2310,17 +2378,20 @@
       <c r="F22" s="2">
         <v>4052702</v>
       </c>
-      <c r="G22" s="2" t="s">
-        <v>159</v>
+      <c r="G22" s="9">
+        <v>942.57999999999993</v>
       </c>
       <c r="H22" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="I22" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="I22" s="2" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J22" s="2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>64</v>
       </c>
@@ -2339,17 +2410,20 @@
       <c r="F23" s="2">
         <v>4050105</v>
       </c>
-      <c r="G23" s="2" t="s">
-        <v>159</v>
+      <c r="G23" s="9">
+        <v>6286.6600000000008</v>
       </c>
       <c r="H23" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="I23" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="I23" s="2" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J23" s="2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>65</v>
       </c>
@@ -2368,17 +2442,20 @@
       <c r="F24" s="2">
         <v>4051764</v>
       </c>
-      <c r="G24" s="2" t="s">
-        <v>159</v>
+      <c r="G24" s="9">
+        <v>1934.79</v>
       </c>
       <c r="H24" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="I24" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="I24" s="2" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J24" s="2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>66</v>
       </c>
@@ -2397,17 +2474,20 @@
       <c r="F25" s="2">
         <v>4051718</v>
       </c>
-      <c r="G25" s="2" t="s">
-        <v>159</v>
+      <c r="G25" s="9">
+        <v>2078.0299999999997</v>
       </c>
       <c r="H25" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="I25" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="I25" s="2" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J25" s="2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>67</v>
       </c>
@@ -2426,17 +2506,20 @@
       <c r="F26" s="2">
         <v>4051804</v>
       </c>
-      <c r="G26" s="2" t="s">
-        <v>159</v>
+      <c r="G26" s="9">
+        <v>2342.58</v>
       </c>
       <c r="H26" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="I26" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="I26" s="2" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J26" s="2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>68</v>
       </c>
@@ -2455,17 +2538,20 @@
       <c r="F27" s="2">
         <v>4051804</v>
       </c>
-      <c r="G27" s="2" t="s">
-        <v>159</v>
+      <c r="G27" s="9">
+        <v>2342.58</v>
       </c>
       <c r="H27" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="I27" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="I27" s="2" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J27" s="2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>69</v>
       </c>
@@ -2484,17 +2570,20 @@
       <c r="F28" s="2">
         <v>4051799</v>
       </c>
-      <c r="G28" s="2" t="s">
-        <v>159</v>
+      <c r="G28" s="9">
+        <v>3168.06</v>
       </c>
       <c r="H28" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="I28" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="I28" s="2" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J28" s="2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>70</v>
       </c>
@@ -2513,17 +2602,20 @@
       <c r="F29" s="2">
         <v>4052905</v>
       </c>
-      <c r="G29" s="2" t="s">
-        <v>159</v>
+      <c r="G29" s="9">
+        <v>659.02</v>
       </c>
       <c r="H29" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="I29" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="I29" s="2" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J29" s="2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>71</v>
       </c>
@@ -2542,17 +2634,20 @@
       <c r="F30" s="2">
         <v>4052882</v>
       </c>
-      <c r="G30" s="2" t="s">
-        <v>159</v>
+      <c r="G30" s="9">
+        <v>681.94999999999993</v>
       </c>
       <c r="H30" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="I30" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="I30" s="2" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J30" s="2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>72</v>
       </c>
@@ -2571,17 +2666,20 @@
       <c r="F31" s="2">
         <v>4052882</v>
       </c>
-      <c r="G31" s="2" t="s">
-        <v>159</v>
+      <c r="G31" s="9">
+        <v>681.94999999999993</v>
       </c>
       <c r="H31" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="I31" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="I31" s="2" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J31" s="2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>73</v>
       </c>
@@ -2600,17 +2698,20 @@
       <c r="F32" s="2">
         <v>4052882</v>
       </c>
-      <c r="G32" s="2" t="s">
-        <v>159</v>
+      <c r="G32" s="9">
+        <v>681.94999999999993</v>
       </c>
       <c r="H32" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="I32" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="I32" s="2" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J32" s="2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>74</v>
       </c>
@@ -2629,17 +2730,20 @@
       <c r="F33" s="2">
         <v>4052882</v>
       </c>
-      <c r="G33" s="2" t="s">
-        <v>159</v>
+      <c r="G33" s="9">
+        <v>681.94999999999993</v>
       </c>
       <c r="H33" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="I33" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="I33" s="2" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J33" s="2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>75</v>
       </c>
@@ -2658,17 +2762,20 @@
       <c r="F34" s="2">
         <v>4052882</v>
       </c>
-      <c r="G34" s="2" t="s">
-        <v>159</v>
+      <c r="G34" s="9">
+        <v>681.94999999999993</v>
       </c>
       <c r="H34" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="I34" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="I34" s="2" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J34" s="2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>76</v>
       </c>
@@ -2687,17 +2794,20 @@
       <c r="F35" s="2">
         <v>4052786</v>
       </c>
-      <c r="G35" s="2" t="s">
-        <v>159</v>
+      <c r="G35" s="9">
+        <v>799.54</v>
       </c>
       <c r="H35" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="I35" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="I35" s="2" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J35" s="2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>77</v>
       </c>
@@ -2716,17 +2826,20 @@
       <c r="F36" s="2">
         <v>4051713</v>
       </c>
-      <c r="G36" s="2" t="s">
-        <v>159</v>
+      <c r="G36" s="9">
+        <v>2078.0299999999997</v>
       </c>
       <c r="H36" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="I36" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="I36" s="2" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J36" s="2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>78</v>
       </c>
@@ -2745,17 +2858,20 @@
       <c r="F37" s="2">
         <v>4051745</v>
       </c>
-      <c r="G37" s="2" t="s">
-        <v>159</v>
+      <c r="G37" s="9">
+        <v>1964.07</v>
       </c>
       <c r="H37" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="I37" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="I37" s="2" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J37" s="2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>79</v>
       </c>
@@ -2774,17 +2890,20 @@
       <c r="F38" s="2">
         <v>4051745</v>
       </c>
-      <c r="G38" s="2" t="s">
-        <v>159</v>
+      <c r="G38" s="9">
+        <v>1964.07</v>
       </c>
       <c r="H38" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="I38" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="I38" s="2" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J38" s="2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>80</v>
       </c>
@@ -2803,17 +2922,20 @@
       <c r="F39" s="2">
         <v>4051093</v>
       </c>
-      <c r="G39" s="2" t="s">
-        <v>159</v>
+      <c r="G39" s="9">
+        <v>4490.25</v>
       </c>
       <c r="H39" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="I39" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="I39" s="2" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J39" s="2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>81</v>
       </c>
@@ -2832,17 +2954,20 @@
       <c r="F40" s="2">
         <v>4052558</v>
       </c>
-      <c r="G40" s="2" t="s">
-        <v>159</v>
+      <c r="G40" s="9">
+        <v>1083.21</v>
       </c>
       <c r="H40" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="I40" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="I40" s="2" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J40" s="2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
         <v>82</v>
       </c>
@@ -2861,17 +2986,20 @@
       <c r="F41" s="2">
         <v>4052558</v>
       </c>
-      <c r="G41" s="2" t="s">
-        <v>159</v>
+      <c r="G41" s="9">
+        <v>1083.21</v>
       </c>
       <c r="H41" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="I41" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="I41" s="2" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J41" s="2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
         <v>83</v>
       </c>
@@ -2890,17 +3018,20 @@
       <c r="F42" s="2">
         <v>4052375</v>
       </c>
-      <c r="G42" s="2" t="s">
-        <v>159</v>
+      <c r="G42" s="9">
+        <v>1295.98</v>
       </c>
       <c r="H42" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="I42" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="I42" s="2" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J42" s="2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
         <v>84</v>
       </c>
@@ -2919,17 +3050,20 @@
       <c r="F43" s="2">
         <v>4052375</v>
       </c>
-      <c r="G43" s="2" t="s">
-        <v>159</v>
+      <c r="G43" s="9">
+        <v>1295.98</v>
       </c>
       <c r="H43" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="I43" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="I43" s="2" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J43" s="2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
         <v>85</v>
       </c>
@@ -2948,17 +3082,20 @@
       <c r="F44" s="2">
         <v>4052375</v>
       </c>
-      <c r="G44" s="2" t="s">
-        <v>159</v>
+      <c r="G44" s="9">
+        <v>1295.98</v>
       </c>
       <c r="H44" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="I44" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="I44" s="2" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J44" s="2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
         <v>86</v>
       </c>
@@ -2977,17 +3114,20 @@
       <c r="F45" s="2">
         <v>4051791</v>
       </c>
-      <c r="G45" s="2" t="s">
-        <v>159</v>
+      <c r="G45" s="9">
+        <v>2318.5099999999998</v>
       </c>
       <c r="H45" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="I45" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="I45" s="2" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J45" s="2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
         <v>87</v>
       </c>
@@ -3006,17 +3146,20 @@
       <c r="F46" s="2">
         <v>4051792</v>
       </c>
-      <c r="G46" s="2" t="s">
-        <v>159</v>
+      <c r="G46" s="9">
+        <v>2318.5099999999998</v>
       </c>
       <c r="H46" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="I46" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="I46" s="2" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J46" s="2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
         <v>88</v>
       </c>
@@ -3035,17 +3178,20 @@
       <c r="F47" s="2">
         <v>4051813</v>
       </c>
-      <c r="G47" s="2" t="s">
-        <v>159</v>
+      <c r="G47" s="9">
+        <v>2349.1799999999998</v>
       </c>
       <c r="H47" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="I47" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="I47" s="2" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J47" s="2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
         <v>89</v>
       </c>
@@ -3064,17 +3210,20 @@
       <c r="F48" s="2">
         <v>4041748</v>
       </c>
-      <c r="G48" s="2" t="s">
-        <v>159</v>
+      <c r="G48" s="9">
+        <v>8613.9700000000012</v>
       </c>
       <c r="H48" s="2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="I48" s="2" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
+        <v>161</v>
+      </c>
+      <c r="J48" s="2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
         <v>90</v>
       </c>
@@ -3093,17 +3242,20 @@
       <c r="F49" s="2">
         <v>4049186</v>
       </c>
-      <c r="G49" s="2" t="s">
-        <v>159</v>
+      <c r="G49" s="9">
+        <v>8613.9700000000012</v>
       </c>
       <c r="H49" s="2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="I49" s="2" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
+        <v>161</v>
+      </c>
+      <c r="J49" s="2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
         <v>91</v>
       </c>
@@ -3122,17 +3274,20 @@
       <c r="F50" s="2">
         <v>4049186</v>
       </c>
-      <c r="G50" s="2" t="s">
-        <v>159</v>
+      <c r="G50" s="9">
+        <v>8613.9700000000012</v>
       </c>
       <c r="H50" s="2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="I50" s="2" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
+        <v>161</v>
+      </c>
+      <c r="J50" s="2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
         <v>92</v>
       </c>
@@ -3151,17 +3306,20 @@
       <c r="F51" s="2">
         <v>4049186</v>
       </c>
-      <c r="G51" s="2" t="s">
-        <v>159</v>
+      <c r="G51" s="9">
+        <v>8613.9700000000012</v>
       </c>
       <c r="H51" s="2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="I51" s="2" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
+        <v>161</v>
+      </c>
+      <c r="J51" s="2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
         <v>93</v>
       </c>
@@ -3180,17 +3338,20 @@
       <c r="F52" s="2">
         <v>4049186</v>
       </c>
-      <c r="G52" s="2" t="s">
-        <v>159</v>
+      <c r="G52" s="9">
+        <v>8613.9700000000012</v>
       </c>
       <c r="H52" s="2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="I52" s="2" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
+        <v>161</v>
+      </c>
+      <c r="J52" s="2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
         <v>94</v>
       </c>
@@ -3209,17 +3370,20 @@
       <c r="F53" s="2">
         <v>4049186</v>
       </c>
-      <c r="G53" s="2" t="s">
-        <v>159</v>
+      <c r="G53" s="9">
+        <v>8613.9700000000012</v>
       </c>
       <c r="H53" s="2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="I53" s="2" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
+        <v>161</v>
+      </c>
+      <c r="J53" s="2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
         <v>95</v>
       </c>
@@ -3238,17 +3402,20 @@
       <c r="F54" s="2">
         <v>4049186</v>
       </c>
-      <c r="G54" s="2" t="s">
-        <v>159</v>
+      <c r="G54" s="9">
+        <v>8613.9700000000012</v>
       </c>
       <c r="H54" s="2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="I54" s="2" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.2">
+        <v>161</v>
+      </c>
+      <c r="J54" s="2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
         <v>96</v>
       </c>
@@ -3267,17 +3434,20 @@
       <c r="F55" s="2">
         <v>4049186</v>
       </c>
-      <c r="G55" s="2" t="s">
-        <v>159</v>
+      <c r="G55" s="9">
+        <v>8613.9700000000012</v>
       </c>
       <c r="H55" s="2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="I55" s="2" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
+        <v>161</v>
+      </c>
+      <c r="J55" s="2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
         <v>97</v>
       </c>
@@ -3296,17 +3466,20 @@
       <c r="F56" s="2">
         <v>4049136</v>
       </c>
-      <c r="G56" s="2" t="s">
-        <v>159</v>
+      <c r="G56" s="9">
+        <v>8613.9700000000012</v>
       </c>
       <c r="H56" s="2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="I56" s="2" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.2">
+        <v>161</v>
+      </c>
+      <c r="J56" s="2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
         <v>98</v>
       </c>
@@ -3325,17 +3498,20 @@
       <c r="F57" s="2">
         <v>4049186</v>
       </c>
-      <c r="G57" s="2" t="s">
-        <v>159</v>
+      <c r="G57" s="9">
+        <v>8613.9700000000012</v>
       </c>
       <c r="H57" s="2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="I57" s="2" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.2">
+        <v>161</v>
+      </c>
+      <c r="J57" s="2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
         <v>99</v>
       </c>
@@ -3354,17 +3530,20 @@
       <c r="F58" s="3">
         <v>4049186</v>
       </c>
-      <c r="G58" s="2" t="s">
-        <v>159</v>
+      <c r="G58" s="9">
+        <v>8613.9700000000012</v>
       </c>
       <c r="H58" s="2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="I58" s="2" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.2">
+        <v>161</v>
+      </c>
+      <c r="J58" s="2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
         <v>100</v>
       </c>
@@ -3383,17 +3562,20 @@
       <c r="F59" s="2">
         <v>4049186</v>
       </c>
-      <c r="G59" s="2" t="s">
-        <v>159</v>
+      <c r="G59" s="9">
+        <v>8613.9700000000012</v>
       </c>
       <c r="H59" s="2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="I59" s="2" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.2">
+        <v>161</v>
+      </c>
+      <c r="J59" s="2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
         <v>101</v>
       </c>
@@ -3412,17 +3594,20 @@
       <c r="F60" s="2">
         <v>4049186</v>
       </c>
-      <c r="G60" s="2" t="s">
-        <v>159</v>
+      <c r="G60" s="9">
+        <v>8613.9700000000012</v>
       </c>
       <c r="H60" s="2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="I60" s="2" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.2">
+        <v>161</v>
+      </c>
+      <c r="J60" s="2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
         <v>102</v>
       </c>
@@ -3441,17 +3626,20 @@
       <c r="F61" s="3">
         <v>4049186</v>
       </c>
-      <c r="G61" s="2" t="s">
-        <v>159</v>
+      <c r="G61" s="9">
+        <v>8613.9700000000012</v>
       </c>
       <c r="H61" s="2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="I61" s="2" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.2">
+        <v>161</v>
+      </c>
+      <c r="J61" s="2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
         <v>103</v>
       </c>
@@ -3470,17 +3658,20 @@
       <c r="F62" s="2">
         <v>4049186</v>
       </c>
-      <c r="G62" s="2" t="s">
-        <v>159</v>
+      <c r="G62" s="9">
+        <v>8613.9700000000012</v>
       </c>
       <c r="H62" s="2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="I62" s="2" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.2">
+        <v>161</v>
+      </c>
+      <c r="J62" s="2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
         <v>104</v>
       </c>
@@ -3499,17 +3690,20 @@
       <c r="F63" s="2">
         <v>4049186</v>
       </c>
-      <c r="G63" s="2" t="s">
-        <v>159</v>
+      <c r="G63" s="9">
+        <v>8613.9700000000012</v>
       </c>
       <c r="H63" s="2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="I63" s="2" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.2">
+        <v>161</v>
+      </c>
+      <c r="J63" s="2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
         <v>105</v>
       </c>
@@ -3528,17 +3722,20 @@
       <c r="F64" s="2">
         <v>4050104</v>
       </c>
-      <c r="G64" s="2" t="s">
-        <v>159</v>
+      <c r="G64" s="9">
+        <v>6317.380000000001</v>
       </c>
       <c r="H64" s="2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="I64" s="2" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.2">
+        <v>161</v>
+      </c>
+      <c r="J64" s="2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
         <v>106</v>
       </c>
@@ -3557,17 +3754,20 @@
       <c r="F65" s="2">
         <v>4050104</v>
       </c>
-      <c r="G65" s="2" t="s">
-        <v>159</v>
+      <c r="G65" s="9">
+        <v>6317.380000000001</v>
       </c>
       <c r="H65" s="2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="I65" s="2" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.2">
+        <v>161</v>
+      </c>
+      <c r="J65" s="2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
         <v>107</v>
       </c>
@@ -3586,17 +3786,20 @@
       <c r="F66" s="2">
         <v>4048631</v>
       </c>
-      <c r="G66" s="2" t="s">
-        <v>159</v>
+      <c r="G66" s="9">
+        <v>12666.370000000004</v>
       </c>
       <c r="H66" s="2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="I66" s="2" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.2">
+        <v>161</v>
+      </c>
+      <c r="J66" s="2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
         <v>108</v>
       </c>
@@ -3615,17 +3818,20 @@
       <c r="F67" s="2">
         <v>4048644</v>
       </c>
-      <c r="G67" s="2" t="s">
-        <v>159</v>
+      <c r="G67" s="9">
+        <v>12734.380000000005</v>
       </c>
       <c r="H67" s="2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="I67" s="2" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.2">
+        <v>161</v>
+      </c>
+      <c r="J67" s="2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
         <v>109</v>
       </c>
@@ -3644,17 +3850,20 @@
       <c r="F68" s="3">
         <v>4048638</v>
       </c>
-      <c r="G68" s="2" t="s">
-        <v>159</v>
+      <c r="G68" s="9">
+        <v>12734.380000000005</v>
       </c>
       <c r="H68" s="2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="I68" s="2" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.2">
+        <v>161</v>
+      </c>
+      <c r="J68" s="2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
         <v>110</v>
       </c>
@@ -3673,17 +3882,20 @@
       <c r="F69" s="2">
         <v>4048661</v>
       </c>
-      <c r="G69" s="2" t="s">
-        <v>159</v>
+      <c r="G69" s="9">
+        <v>12967.650000000005</v>
       </c>
       <c r="H69" s="2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="I69" s="2" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.2">
+        <v>161</v>
+      </c>
+      <c r="J69" s="2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
         <v>111</v>
       </c>
@@ -3702,17 +3914,20 @@
       <c r="F70" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="G70" s="2" t="s">
-        <v>159</v>
+      <c r="G70" s="9">
+        <v>13944.970000000007</v>
       </c>
       <c r="H70" s="2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="I70" s="2" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.2">
+        <v>161</v>
+      </c>
+      <c r="J70" s="2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
         <v>112</v>
       </c>
@@ -3731,17 +3946,20 @@
       <c r="F71" s="2">
         <v>4048793</v>
       </c>
-      <c r="G71" s="2" t="s">
-        <v>159</v>
+      <c r="G71" s="9">
+        <v>13944.970000000007</v>
       </c>
       <c r="H71" s="2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="I71" s="2" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.2">
+        <v>161</v>
+      </c>
+      <c r="J71" s="2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="72" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
         <v>113</v>
       </c>
@@ -3760,17 +3978,20 @@
       <c r="F72" s="2">
         <v>4048635</v>
       </c>
-      <c r="G72" s="2" t="s">
-        <v>159</v>
+      <c r="G72" s="9">
+        <v>14312.610000000006</v>
       </c>
       <c r="H72" s="2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="I72" s="2" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.2">
+        <v>161</v>
+      </c>
+      <c r="J72" s="2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
         <v>114</v>
       </c>
@@ -3789,17 +4010,20 @@
       <c r="F73" s="2">
         <v>4049469</v>
       </c>
-      <c r="G73" s="2" t="s">
-        <v>159</v>
+      <c r="G73" s="9">
+        <v>15837.420000000006</v>
       </c>
       <c r="H73" s="2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="I73" s="2" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.2">
+        <v>161</v>
+      </c>
+      <c r="J73" s="2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="74" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
         <v>115</v>
       </c>
@@ -3818,17 +4042,20 @@
       <c r="F74" s="2">
         <v>4048721</v>
       </c>
-      <c r="G74" s="2" t="s">
-        <v>159</v>
+      <c r="G74" s="9">
+        <v>13192.270000000006</v>
       </c>
       <c r="H74" s="2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="I74" s="2" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.2">
+        <v>161</v>
+      </c>
+      <c r="J74" s="2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="75" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A75" s="1" t="s">
         <v>116</v>
       </c>
@@ -3847,17 +4074,20 @@
       <c r="F75" s="2">
         <v>4049790</v>
       </c>
-      <c r="G75" s="2" t="s">
-        <v>159</v>
+      <c r="G75" s="9">
+        <v>7600.5100000000011</v>
       </c>
       <c r="H75" s="2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="I75" s="2" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.2">
+        <v>161</v>
+      </c>
+      <c r="J75" s="2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="s">
         <v>117</v>
       </c>
@@ -3876,17 +4106,20 @@
       <c r="F76" s="2">
         <v>4050181</v>
       </c>
-      <c r="G76" s="2" t="s">
-        <v>159</v>
+      <c r="G76" s="9">
+        <v>17031.800000000007</v>
       </c>
       <c r="H76" s="2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="I76" s="2" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.2">
+        <v>161</v>
+      </c>
+      <c r="J76" s="2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A77" s="1" t="s">
         <v>118</v>
       </c>
@@ -3905,17 +4138,20 @@
       <c r="F77" s="2">
         <v>4049626</v>
       </c>
-      <c r="G77" s="2" t="s">
-        <v>159</v>
+      <c r="G77" s="9">
+        <v>17916.28000000001</v>
       </c>
       <c r="H77" s="2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="I77" s="2" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.2">
+        <v>161</v>
+      </c>
+      <c r="J77" s="2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="s">
         <v>119</v>
       </c>
@@ -3934,17 +4170,20 @@
       <c r="F78" s="2">
         <v>4050015</v>
       </c>
-      <c r="G78" s="2" t="s">
-        <v>159</v>
+      <c r="G78" s="9">
+        <v>7056.8500000000013</v>
       </c>
       <c r="H78" s="2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="I78" s="2" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.2">
+        <v>161</v>
+      </c>
+      <c r="J78" s="2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
         <v>120</v>
       </c>
@@ -3963,17 +4202,20 @@
       <c r="F79" s="2">
         <v>4049528</v>
       </c>
-      <c r="G79" s="2" t="s">
-        <v>159</v>
+      <c r="G79" s="9">
+        <v>8053.1100000000015</v>
       </c>
       <c r="H79" s="2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="I79" s="2" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.2">
+        <v>161</v>
+      </c>
+      <c r="J79" s="2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
         <v>121</v>
       </c>
@@ -3992,17 +4234,20 @@
       <c r="F80" s="2">
         <v>4049186</v>
       </c>
-      <c r="G80" s="2" t="s">
-        <v>159</v>
+      <c r="G80" s="9">
+        <v>9082.880000000001</v>
       </c>
       <c r="H80" s="2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="I80" s="2" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.2">
+        <v>161</v>
+      </c>
+      <c r="J80" s="2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A81" s="1" t="s">
         <v>122</v>
       </c>
@@ -4021,17 +4266,20 @@
       <c r="F81" s="2">
         <v>4048313</v>
       </c>
-      <c r="G81" s="2" t="s">
-        <v>159</v>
+      <c r="G81" s="9">
+        <v>10462.430000000002</v>
       </c>
       <c r="H81" s="2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="I81" s="2" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.2">
+        <v>161</v>
+      </c>
+      <c r="J81" s="2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A82" s="1" t="s">
         <v>123</v>
       </c>
@@ -4050,17 +4298,20 @@
       <c r="F82" s="2">
         <v>4048313</v>
       </c>
-      <c r="G82" s="2" t="s">
-        <v>159</v>
+      <c r="G82" s="9">
+        <v>10462.430000000002</v>
       </c>
       <c r="H82" s="2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="I82" s="2" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.2">
+        <v>161</v>
+      </c>
+      <c r="J82" s="2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A83" s="1" t="s">
         <v>124</v>
       </c>
@@ -4079,17 +4330,20 @@
       <c r="F83" s="2">
         <v>4048313</v>
       </c>
-      <c r="G83" s="2" t="s">
-        <v>159</v>
+      <c r="G83" s="9">
+        <v>10462.430000000002</v>
       </c>
       <c r="H83" s="2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="I83" s="2" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.2">
+        <v>161</v>
+      </c>
+      <c r="J83" s="2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A84" s="1" t="s">
         <v>125</v>
       </c>
@@ -4108,17 +4362,20 @@
       <c r="F84" s="2">
         <v>4047966</v>
       </c>
-      <c r="G84" s="2" t="s">
-        <v>159</v>
+      <c r="G84" s="9">
+        <v>10929.640000000003</v>
       </c>
       <c r="H84" s="2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="I84" s="2" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.2">
+        <v>161</v>
+      </c>
+      <c r="J84" s="2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A85" s="1" t="s">
         <v>126</v>
       </c>
@@ -4137,17 +4394,20 @@
       <c r="F85" s="2">
         <v>4047966</v>
       </c>
-      <c r="G85" s="2" t="s">
-        <v>159</v>
+      <c r="G85" s="9">
+        <v>10929.640000000003</v>
       </c>
       <c r="H85" s="2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="I85" s="2" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.2">
+        <v>161</v>
+      </c>
+      <c r="J85" s="2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A86" s="1" t="s">
         <v>127</v>
       </c>
@@ -4166,17 +4426,20 @@
       <c r="F86" s="2">
         <v>4047930</v>
       </c>
-      <c r="G86" s="2" t="s">
-        <v>159</v>
+      <c r="G86" s="9">
+        <v>11139.010000000004</v>
       </c>
       <c r="H86" s="2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="I86" s="2" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.2">
+        <v>161</v>
+      </c>
+      <c r="J86" s="2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A87" s="1" t="s">
         <v>128</v>
       </c>
@@ -4195,17 +4458,20 @@
       <c r="F87" s="2">
         <v>4050111</v>
       </c>
-      <c r="G87" s="2" t="s">
-        <v>159</v>
+      <c r="G87" s="9">
+        <v>17360.310000000009</v>
       </c>
       <c r="H87" s="2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="I87" s="2" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.2">
+        <v>161</v>
+      </c>
+      <c r="J87" s="2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A88" s="1" t="s">
         <v>129</v>
       </c>
@@ -4224,17 +4490,20 @@
       <c r="F88" s="2">
         <v>4050090</v>
       </c>
-      <c r="G88" s="2" t="s">
-        <v>159</v>
+      <c r="G88" s="9">
+        <v>17423.89000000001</v>
       </c>
       <c r="H88" s="2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="I88" s="2" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.2">
+        <v>161</v>
+      </c>
+      <c r="J88" s="2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A89" s="1" t="s">
         <v>130</v>
       </c>
@@ -4253,17 +4522,20 @@
       <c r="F89" s="2">
         <v>4049744</v>
       </c>
-      <c r="G89" s="2" t="s">
-        <v>159</v>
+      <c r="G89" s="9">
+        <v>16280.420000000006</v>
       </c>
       <c r="H89" s="2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="I89" s="2" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.2">
+        <v>161</v>
+      </c>
+      <c r="J89" s="2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="90" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A90" s="1" t="s">
         <v>131</v>
       </c>
@@ -4282,17 +4554,20 @@
       <c r="F90" s="2">
         <v>4050208</v>
       </c>
-      <c r="G90" s="2" t="s">
-        <v>159</v>
+      <c r="G90" s="9">
+        <v>17113.410000000007</v>
       </c>
       <c r="H90" s="2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="I90" s="2" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.2">
+        <v>161</v>
+      </c>
+      <c r="J90" s="2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="91" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A91" s="1" t="s">
         <v>132</v>
       </c>
@@ -4311,17 +4586,20 @@
       <c r="F91" s="2">
         <v>4048202</v>
       </c>
-      <c r="G91" s="2" t="s">
-        <v>159</v>
+      <c r="G91" s="9">
+        <v>10655.960000000003</v>
       </c>
       <c r="H91" s="2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="I91" s="2" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.2">
+        <v>161</v>
+      </c>
+      <c r="J91" s="2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="92" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A92" s="1" t="s">
         <v>133</v>
       </c>
@@ -4340,17 +4618,20 @@
       <c r="F92" s="2">
         <v>4048318</v>
       </c>
-      <c r="G92" s="2" t="s">
-        <v>159</v>
+      <c r="G92" s="9">
+        <v>10462.430000000002</v>
       </c>
       <c r="H92" s="2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="I92" s="2" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.2">
+        <v>161</v>
+      </c>
+      <c r="J92" s="2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="93" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A93" s="1" t="s">
         <v>134</v>
       </c>
@@ -4369,17 +4650,20 @@
       <c r="F93" s="2">
         <v>4049067</v>
       </c>
-      <c r="G93" s="2" t="s">
-        <v>159</v>
+      <c r="G93" s="9">
+        <v>9395.4700000000012</v>
       </c>
       <c r="H93" s="2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="I93" s="2" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.2">
+        <v>161</v>
+      </c>
+      <c r="J93" s="2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="94" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A94" s="1" t="s">
         <v>135</v>
       </c>
@@ -4398,17 +4682,20 @@
       <c r="F94" s="2">
         <v>4049649</v>
       </c>
-      <c r="G94" s="2" t="s">
-        <v>159</v>
+      <c r="G94" s="9">
+        <v>7868.4400000000014</v>
       </c>
       <c r="H94" s="2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="I94" s="2" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.2">
+        <v>161</v>
+      </c>
+      <c r="J94" s="2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="95" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A95" s="1" t="s">
         <v>136</v>
       </c>
@@ -4427,17 +4714,20 @@
       <c r="F95" s="2">
         <v>4050015</v>
       </c>
-      <c r="G95" s="2" t="s">
-        <v>159</v>
+      <c r="G95" s="9">
+        <v>7056.8500000000013</v>
       </c>
       <c r="H95" s="2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="I95" s="2" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.2">
+        <v>161</v>
+      </c>
+      <c r="J95" s="2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="96" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A96" s="1" t="s">
         <v>137</v>
       </c>
@@ -4456,17 +4746,20 @@
       <c r="F96" s="2">
         <v>4050015</v>
       </c>
-      <c r="G96" s="2" t="s">
-        <v>159</v>
+      <c r="G96" s="9">
+        <v>7056.8500000000013</v>
       </c>
       <c r="H96" s="2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="I96" s="2" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.2">
+        <v>161</v>
+      </c>
+      <c r="J96" s="2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="97" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A97" s="1" t="s">
         <v>138</v>
       </c>
@@ -4485,17 +4778,20 @@
       <c r="F97" s="2">
         <v>4049239</v>
       </c>
-      <c r="G97" s="2" t="s">
-        <v>159</v>
+      <c r="G97" s="9">
+        <v>8463.8000000000011</v>
       </c>
       <c r="H97" s="2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="I97" s="2" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.2">
+        <v>161</v>
+      </c>
+      <c r="J97" s="2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="98" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A98" s="1" t="s">
         <v>139</v>
       </c>
@@ -4514,17 +4810,20 @@
       <c r="F98" s="2">
         <v>4049239</v>
       </c>
-      <c r="G98" s="2" t="s">
-        <v>159</v>
+      <c r="G98" s="9">
+        <v>8463.8000000000011</v>
       </c>
       <c r="H98" s="2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="I98" s="2" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.2">
+        <v>161</v>
+      </c>
+      <c r="J98" s="2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="99" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A99" s="1" t="s">
         <v>140</v>
       </c>
@@ -4543,17 +4842,20 @@
       <c r="F99" s="2">
         <v>4049178</v>
       </c>
-      <c r="G99" s="2" t="s">
-        <v>159</v>
+      <c r="G99" s="9">
+        <v>9082.880000000001</v>
       </c>
       <c r="H99" s="2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="I99" s="2" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.2">
+        <v>161</v>
+      </c>
+      <c r="J99" s="2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="100" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A100" s="1" t="s">
         <v>141</v>
       </c>
@@ -4572,17 +4874,20 @@
       <c r="F100" s="2">
         <v>4049178</v>
       </c>
-      <c r="G100" s="2" t="s">
-        <v>159</v>
+      <c r="G100" s="9">
+        <v>9082.880000000001</v>
       </c>
       <c r="H100" s="2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="I100" s="2" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="101" spans="1:9" x14ac:dyDescent="0.2">
+        <v>161</v>
+      </c>
+      <c r="J100" s="2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="101" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A101" s="1" t="s">
         <v>142</v>
       </c>
@@ -4601,17 +4906,20 @@
       <c r="F101" s="2">
         <v>4049178</v>
       </c>
-      <c r="G101" s="2" t="s">
-        <v>159</v>
+      <c r="G101" s="9">
+        <v>9082.880000000001</v>
       </c>
       <c r="H101" s="2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="I101" s="2" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="102" spans="1:9" x14ac:dyDescent="0.2">
+        <v>161</v>
+      </c>
+      <c r="J101" s="2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="102" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A102" s="1" t="s">
         <v>143</v>
       </c>
@@ -4630,17 +4938,20 @@
       <c r="F102" s="2">
         <v>4049178</v>
       </c>
-      <c r="G102" s="2" t="s">
-        <v>159</v>
+      <c r="G102" s="9">
+        <v>9082.880000000001</v>
       </c>
       <c r="H102" s="2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="I102" s="2" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="103" spans="1:9" x14ac:dyDescent="0.2">
+        <v>161</v>
+      </c>
+      <c r="J102" s="2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="103" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A103" s="1" t="s">
         <v>144</v>
       </c>
@@ -4659,17 +4970,20 @@
       <c r="F103" s="2">
         <v>4049178</v>
       </c>
-      <c r="G103" s="2" t="s">
-        <v>159</v>
+      <c r="G103" s="9">
+        <v>9082.880000000001</v>
       </c>
       <c r="H103" s="2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="I103" s="2" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="104" spans="1:9" x14ac:dyDescent="0.2">
+        <v>161</v>
+      </c>
+      <c r="J103" s="2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="104" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A104" s="1" t="s">
         <v>145</v>
       </c>
@@ -4688,17 +5002,20 @@
       <c r="F104" s="2">
         <v>4049178</v>
       </c>
-      <c r="G104" s="2" t="s">
-        <v>159</v>
+      <c r="G104" s="9">
+        <v>9082.880000000001</v>
       </c>
       <c r="H104" s="2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="I104" s="2" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="105" spans="1:9" x14ac:dyDescent="0.2">
+        <v>161</v>
+      </c>
+      <c r="J104" s="2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="105" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A105" s="1" t="s">
         <v>146</v>
       </c>
@@ -4717,17 +5034,20 @@
       <c r="F105" s="2">
         <v>4048916</v>
       </c>
-      <c r="G105" s="2" t="s">
-        <v>159</v>
+      <c r="G105" s="9">
+        <v>9583.510000000002</v>
       </c>
       <c r="H105" s="2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="I105" s="2" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="106" spans="1:9" x14ac:dyDescent="0.2">
+        <v>161</v>
+      </c>
+      <c r="J105" s="2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="106" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A106" s="1" t="s">
         <v>147</v>
       </c>
@@ -4746,17 +5066,20 @@
       <c r="F106" s="2">
         <v>4048646</v>
       </c>
-      <c r="G106" s="2" t="s">
-        <v>159</v>
+      <c r="G106" s="9">
+        <v>10074.350000000002</v>
       </c>
       <c r="H106" s="2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="I106" s="2" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="107" spans="1:9" x14ac:dyDescent="0.2">
+        <v>161</v>
+      </c>
+      <c r="J106" s="2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="107" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A107" s="1" t="s">
         <v>148</v>
       </c>
@@ -4775,17 +5098,20 @@
       <c r="F107" s="2">
         <v>4048426</v>
       </c>
-      <c r="G107" s="2" t="s">
-        <v>159</v>
+      <c r="G107" s="9">
+        <v>10298.670000000002</v>
       </c>
       <c r="H107" s="2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="I107" s="2" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="108" spans="1:9" x14ac:dyDescent="0.2">
+        <v>161</v>
+      </c>
+      <c r="J107" s="2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="108" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A108" s="1" t="s">
         <v>149</v>
       </c>
@@ -4804,17 +5130,20 @@
       <c r="F108" s="2">
         <v>4049239</v>
       </c>
-      <c r="G108" s="2" t="s">
-        <v>159</v>
+      <c r="G108" s="9">
+        <v>8463.8000000000011</v>
       </c>
       <c r="H108" s="2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="I108" s="2" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="109" spans="1:9" x14ac:dyDescent="0.2">
+        <v>161</v>
+      </c>
+      <c r="J108" s="2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="109" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A109" s="1" t="s">
         <v>150</v>
       </c>
@@ -4833,17 +5162,20 @@
       <c r="F109" s="2">
         <v>4050021</v>
       </c>
-      <c r="G109" s="2" t="s">
-        <v>159</v>
+      <c r="G109" s="9">
+        <v>6960.1000000000013</v>
       </c>
       <c r="H109" s="2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="I109" s="2" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="110" spans="1:9" x14ac:dyDescent="0.2">
+        <v>161</v>
+      </c>
+      <c r="J109" s="2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="110" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A110" s="1" t="s">
         <v>151</v>
       </c>
@@ -4862,17 +5194,20 @@
       <c r="F110" s="2">
         <v>4050029</v>
       </c>
-      <c r="G110" s="2" t="s">
-        <v>159</v>
+      <c r="G110" s="9">
+        <v>6960.1000000000013</v>
       </c>
       <c r="H110" s="2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="I110" s="2" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="111" spans="1:9" x14ac:dyDescent="0.2">
+        <v>161</v>
+      </c>
+      <c r="J110" s="2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="111" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A111" s="1" t="s">
         <v>152</v>
       </c>
@@ -4891,17 +5226,20 @@
       <c r="F111" s="2">
         <v>4050011</v>
       </c>
-      <c r="G111" s="2" t="s">
-        <v>159</v>
+      <c r="G111" s="9">
+        <v>7025.9000000000015</v>
       </c>
       <c r="H111" s="2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="I111" s="2" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="112" spans="1:9" x14ac:dyDescent="0.2">
+        <v>161</v>
+      </c>
+      <c r="J111" s="2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="112" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A112" s="1" t="s">
         <v>153</v>
       </c>
@@ -4920,17 +5258,20 @@
       <c r="F112" s="2">
         <v>4050011</v>
       </c>
-      <c r="G112" s="2" t="s">
-        <v>159</v>
+      <c r="G112" s="9">
+        <v>7025.9000000000015</v>
       </c>
       <c r="H112" s="2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="I112" s="2" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="113" spans="1:9" x14ac:dyDescent="0.2">
+        <v>161</v>
+      </c>
+      <c r="J112" s="2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="113" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A113" s="1" t="s">
         <v>154</v>
       </c>
@@ -4949,17 +5290,20 @@
       <c r="F113" s="2">
         <v>4050011</v>
       </c>
-      <c r="G113" s="2" t="s">
-        <v>159</v>
+      <c r="G113" s="9">
+        <v>7025.9000000000015</v>
       </c>
       <c r="H113" s="2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="I113" s="2" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="114" spans="1:9" x14ac:dyDescent="0.2">
+        <v>161</v>
+      </c>
+      <c r="J113" s="2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="114" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A114" s="1" t="s">
         <v>155</v>
       </c>
@@ -4978,17 +5322,20 @@
       <c r="F114" s="2">
         <v>4050010</v>
       </c>
-      <c r="G114" s="2" t="s">
-        <v>159</v>
+      <c r="G114" s="9">
+        <v>7025.9000000000015</v>
       </c>
       <c r="H114" s="2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="I114" s="2" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="115" spans="1:9" x14ac:dyDescent="0.2">
+        <v>161</v>
+      </c>
+      <c r="J114" s="2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="115" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A115" s="1" t="s">
         <v>156</v>
       </c>
@@ -5007,17 +5354,20 @@
       <c r="F115" s="2">
         <v>4050003</v>
       </c>
-      <c r="G115" s="2" t="s">
-        <v>159</v>
+      <c r="G115" s="9">
+        <v>7262.6000000000013</v>
       </c>
       <c r="H115" s="2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="I115" s="2" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="116" spans="1:9" x14ac:dyDescent="0.2">
+        <v>161</v>
+      </c>
+      <c r="J115" s="2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="116" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A116" s="1" t="s">
         <v>157</v>
       </c>
@@ -5036,17 +5386,20 @@
       <c r="F116" s="2">
         <v>4050003</v>
       </c>
-      <c r="G116" s="2" t="s">
-        <v>159</v>
+      <c r="G116" s="9">
+        <v>7262.6000000000013</v>
       </c>
       <c r="H116" s="2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="I116" s="2" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="117" spans="1:9" x14ac:dyDescent="0.2">
+        <v>161</v>
+      </c>
+      <c r="J116" s="2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="117" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A117" s="1" t="s">
         <v>158</v>
       </c>
@@ -5065,17 +5418,20 @@
       <c r="F117" s="2">
         <v>4050015</v>
       </c>
-      <c r="G117" s="2" t="s">
-        <v>159</v>
+      <c r="G117" s="9">
+        <v>7056.8500000000013</v>
       </c>
       <c r="H117" s="2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="I117" s="2" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="118" spans="1:9" x14ac:dyDescent="0.2">
+        <v>161</v>
+      </c>
+      <c r="J117" s="2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="118" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A118" s="1" t="s">
         <v>238</v>
       </c>
@@ -5094,17 +5450,17 @@
       <c r="F118" t="s">
         <v>165</v>
       </c>
-      <c r="G118" s="2" t="s">
+      <c r="H118" s="2" t="s">
         <v>240</v>
       </c>
-      <c r="H118" s="2" t="s">
+      <c r="I118" s="2" t="s">
         <v>241</v>
       </c>
-      <c r="I118" s="2" t="s">
+      <c r="J118" s="2" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="119" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A119" s="1" t="s">
         <v>243</v>
       </c>
@@ -5123,17 +5479,17 @@
       <c r="F119" t="s">
         <v>165</v>
       </c>
-      <c r="G119" s="2" t="s">
+      <c r="H119" s="2" t="s">
         <v>240</v>
       </c>
-      <c r="H119" s="2" t="s">
+      <c r="I119" s="2" t="s">
         <v>241</v>
       </c>
-      <c r="I119" s="2" t="s">
+      <c r="J119" s="2" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="120" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A120" s="1" t="s">
         <v>244</v>
       </c>
@@ -5152,17 +5508,17 @@
       <c r="F120" t="s">
         <v>165</v>
       </c>
-      <c r="G120" s="2" t="s">
+      <c r="H120" s="2" t="s">
         <v>240</v>
       </c>
-      <c r="H120" s="2" t="s">
+      <c r="I120" s="2" t="s">
         <v>241</v>
       </c>
-      <c r="I120" s="2" t="s">
+      <c r="J120" s="2" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="121" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A121" s="1" t="s">
         <v>245</v>
       </c>
@@ -5181,17 +5537,17 @@
       <c r="F121" t="s">
         <v>165</v>
       </c>
-      <c r="G121" s="2" t="s">
+      <c r="H121" s="2" t="s">
         <v>240</v>
       </c>
-      <c r="H121" s="2" t="s">
+      <c r="I121" s="2" t="s">
         <v>241</v>
       </c>
-      <c r="I121" s="2" t="s">
+      <c r="J121" s="2" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="122" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A122" s="1" t="s">
         <v>246</v>
       </c>
@@ -5210,17 +5566,17 @@
       <c r="F122" t="s">
         <v>165</v>
       </c>
-      <c r="G122" s="2" t="s">
+      <c r="H122" s="2" t="s">
         <v>240</v>
       </c>
-      <c r="H122" s="2" t="s">
+      <c r="I122" s="2" t="s">
         <v>241</v>
       </c>
-      <c r="I122" s="2" t="s">
+      <c r="J122" s="2" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="123" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A123" s="1" t="s">
         <v>247</v>
       </c>
@@ -5239,17 +5595,17 @@
       <c r="F123" t="s">
         <v>165</v>
       </c>
-      <c r="G123" s="2" t="s">
+      <c r="H123" s="2" t="s">
         <v>240</v>
       </c>
-      <c r="H123" s="2" t="s">
+      <c r="I123" s="2" t="s">
         <v>241</v>
       </c>
-      <c r="I123" s="2" t="s">
+      <c r="J123" s="2" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="124" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A124" s="1" t="s">
         <v>248</v>
       </c>
@@ -5268,17 +5624,17 @@
       <c r="F124" t="s">
         <v>165</v>
       </c>
-      <c r="G124" s="2" t="s">
+      <c r="H124" s="2" t="s">
         <v>240</v>
       </c>
-      <c r="H124" s="2" t="s">
+      <c r="I124" s="2" t="s">
         <v>241</v>
       </c>
-      <c r="I124" s="2" t="s">
+      <c r="J124" s="2" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="125" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A125" s="1" t="s">
         <v>249</v>
       </c>
@@ -5297,17 +5653,17 @@
       <c r="F125" t="s">
         <v>165</v>
       </c>
-      <c r="G125" s="2" t="s">
+      <c r="H125" s="2" t="s">
         <v>240</v>
       </c>
-      <c r="H125" s="2" t="s">
+      <c r="I125" s="2" t="s">
         <v>250</v>
       </c>
-      <c r="I125" s="2" t="s">
+      <c r="J125" s="2" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="126" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A126" s="1" t="s">
         <v>251</v>
       </c>
@@ -5326,17 +5682,17 @@
       <c r="F126" t="s">
         <v>165</v>
       </c>
-      <c r="G126" s="2" t="s">
+      <c r="H126" s="2" t="s">
         <v>240</v>
       </c>
-      <c r="H126" s="2" t="s">
+      <c r="I126" s="2" t="s">
         <v>250</v>
       </c>
-      <c r="I126" s="2" t="s">
+      <c r="J126" s="2" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="127" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A127" s="1" t="s">
         <v>252</v>
       </c>
@@ -5355,17 +5711,17 @@
       <c r="F127" t="s">
         <v>165</v>
       </c>
-      <c r="G127" s="2" t="s">
+      <c r="H127" s="2" t="s">
         <v>240</v>
       </c>
-      <c r="H127" s="2" t="s">
+      <c r="I127" s="2" t="s">
         <v>241</v>
       </c>
-      <c r="I127" s="2" t="s">
+      <c r="J127" s="2" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="128" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A128" s="1" t="s">
         <v>253</v>
       </c>
@@ -5384,17 +5740,17 @@
       <c r="F128" t="s">
         <v>165</v>
       </c>
-      <c r="G128" s="2" t="s">
+      <c r="H128" s="2" t="s">
         <v>240</v>
       </c>
-      <c r="H128" s="2" t="s">
+      <c r="I128" s="2" t="s">
         <v>241</v>
       </c>
-      <c r="I128" s="2" t="s">
+      <c r="J128" s="2" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="129" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A129" s="1" t="s">
         <v>254</v>
       </c>
@@ -5413,17 +5769,17 @@
       <c r="F129" t="s">
         <v>165</v>
       </c>
-      <c r="G129" s="2" t="s">
+      <c r="H129" s="2" t="s">
         <v>240</v>
       </c>
-      <c r="H129" s="2" t="s">
+      <c r="I129" s="2" t="s">
         <v>241</v>
       </c>
-      <c r="I129" s="2" t="s">
+      <c r="J129" s="2" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="130" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A130" s="1" t="s">
         <v>255</v>
       </c>
@@ -5442,17 +5798,17 @@
       <c r="F130" t="s">
         <v>165</v>
       </c>
-      <c r="G130" s="2" t="s">
+      <c r="H130" s="2" t="s">
         <v>240</v>
       </c>
-      <c r="H130" s="2" t="s">
+      <c r="I130" s="2" t="s">
         <v>257</v>
       </c>
-      <c r="I130" s="2" t="s">
+      <c r="J130" s="2" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="131" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A131" s="1" t="s">
         <v>258</v>
       </c>
@@ -5471,17 +5827,17 @@
       <c r="F131" t="s">
         <v>165</v>
       </c>
-      <c r="G131" s="2" t="s">
+      <c r="H131" s="2" t="s">
         <v>240</v>
       </c>
-      <c r="H131" s="2" t="s">
+      <c r="I131" s="2" t="s">
         <v>257</v>
       </c>
-      <c r="I131" s="2" t="s">
+      <c r="J131" s="2" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="132" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A132" s="1" t="s">
         <v>259</v>
       </c>
@@ -5500,17 +5856,17 @@
       <c r="F132" t="s">
         <v>165</v>
       </c>
-      <c r="G132" s="2" t="s">
+      <c r="H132" s="2" t="s">
         <v>240</v>
       </c>
-      <c r="H132" s="2" t="s">
+      <c r="I132" s="2" t="s">
         <v>257</v>
       </c>
-      <c r="I132" s="2" t="s">
+      <c r="J132" s="2" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="133" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A133" s="1" t="s">
         <v>260</v>
       </c>
@@ -5529,17 +5885,17 @@
       <c r="F133" t="s">
         <v>165</v>
       </c>
-      <c r="G133" s="2" t="s">
+      <c r="H133" s="2" t="s">
         <v>240</v>
       </c>
-      <c r="H133" s="2" t="s">
+      <c r="I133" s="2" t="s">
         <v>257</v>
       </c>
-      <c r="I133" s="2" t="s">
+      <c r="J133" s="2" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="134" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A134" s="1" t="s">
         <v>261</v>
       </c>
@@ -5558,17 +5914,17 @@
       <c r="F134" t="s">
         <v>165</v>
       </c>
-      <c r="G134" s="2" t="s">
+      <c r="H134" s="2" t="s">
         <v>240</v>
       </c>
-      <c r="H134" s="2" t="s">
+      <c r="I134" s="2" t="s">
         <v>257</v>
       </c>
-      <c r="I134" s="2" t="s">
+      <c r="J134" s="2" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="135" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A135" s="1" t="s">
         <v>262</v>
       </c>
@@ -5587,17 +5943,17 @@
       <c r="F135" t="s">
         <v>165</v>
       </c>
-      <c r="G135" s="2" t="s">
+      <c r="H135" s="2" t="s">
         <v>240</v>
       </c>
-      <c r="H135" s="2" t="s">
+      <c r="I135" s="2" t="s">
         <v>257</v>
       </c>
-      <c r="I135" s="2" t="s">
+      <c r="J135" s="2" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="136" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A136" s="1" t="s">
         <v>263</v>
       </c>
@@ -5616,17 +5972,17 @@
       <c r="F136" t="s">
         <v>165</v>
       </c>
-      <c r="G136" s="2" t="s">
+      <c r="H136" s="2" t="s">
         <v>240</v>
       </c>
-      <c r="H136" s="2" t="s">
+      <c r="I136" s="2" t="s">
         <v>257</v>
       </c>
-      <c r="I136" s="2" t="s">
+      <c r="J136" s="2" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="137" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A137" s="1" t="s">
         <v>264</v>
       </c>
@@ -5645,13 +6001,13 @@
       <c r="F137" t="s">
         <v>165</v>
       </c>
-      <c r="G137" s="2" t="s">
+      <c r="H137" s="2" t="s">
         <v>240</v>
       </c>
-      <c r="H137" s="2" t="s">
+      <c r="I137" s="2" t="s">
         <v>257</v>
       </c>
-      <c r="I137" s="2" t="s">
+      <c r="J137" s="2" t="s">
         <v>242</v>
       </c>
     </row>

</xml_diff>